<commit_message>
tolte dispense modifica DT dati
</commit_message>
<xml_diff>
--- a/Shiny/Dati/Collirio_2waov.xlsx
+++ b/Shiny/Dati/Collirio_2waov.xlsx
@@ -21,9 +21,6 @@
     <t>Preparazione</t>
   </si>
   <si>
-    <t>lotto</t>
-  </si>
-  <si>
     <t>Pesata</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>A10s</t>
+  </si>
+  <si>
+    <t>Lotto</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C33"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -401,15 +401,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>2150</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>2150</v>
@@ -431,7 +431,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>2150</v>
@@ -442,7 +442,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>2150</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>2151</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
         <v>2151</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2">
         <v>2151</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2">
         <v>2151</v>
@@ -497,7 +497,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2">
         <v>2150</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2">
         <v>2150</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2">
         <v>2150</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2">
         <v>2150</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="2">
         <v>2151</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2">
         <v>2151</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="2">
         <v>2151</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="2">
         <v>2151</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2">
         <v>2150</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2">
         <v>2150</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="2">
         <v>2150</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="2">
         <v>2150</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2">
         <v>2151</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="2">
         <v>2151</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="2">
         <v>2151</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="2">
         <v>2151</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2">
         <v>2150</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2">
         <v>2150</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2">
         <v>2150</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2">
         <v>2150</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="2">
         <v>2151</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="2">
         <v>2151</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" s="2">
         <v>2151</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" s="2">
         <v>2151</v>

</xml_diff>